<commit_message>
changed directory structure; updated structure of procedure file; updated assembly to take in one row instead of processing entire excel file
</commit_message>
<xml_diff>
--- a/Data/imagemap.xlsx
+++ b/Data/imagemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andywang/Desktop/Learning Behavior/Aliens/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B810C-4977-AE42-B3AD-E6150E62C986}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F2ABA3-1CBE-6544-B45F-8510F952AAF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="16940" xr2:uid="{BD53F7A6-3B44-6D46-90D6-01272792EFD4}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>Data/Images/2_body.png</t>
   </si>
   <si>
-    <t>Data/Images/1_body.png</t>
-  </si>
-  <si>
     <t>2_tail_1</t>
   </si>
   <si>
@@ -261,42 +258,6 @@
     <t>1_mou_5</t>
   </si>
   <si>
-    <t>Data/Images/1_arm_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_leg_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_arm_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_arm_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_arm_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_arm_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_leg_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_leg_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_leg_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_leg_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_eye_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_eye_2.png</t>
-  </si>
-  <si>
     <t>Data/Images/1_eye_3.png</t>
   </si>
   <si>
@@ -502,6 +463,45 @@
   </si>
   <si>
     <t>Data/Images/2_tail_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_body.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_arm_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_arm_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_arm_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_arm_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_arm_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_leg_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_leg_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_leg_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_leg_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_leg_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_eye_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_eye_2.png</t>
   </si>
 </sst>
 </file>
@@ -862,13 +862,13 @@
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -927,207 +927,207 @@
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1220,250 +1220,250 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B60" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed parameters of get_alien
</commit_message>
<xml_diff>
--- a/Data/imagemap.xlsx
+++ b/Data/imagemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andywang/Desktop/Learning Behavior/Aliens/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F2ABA3-1CBE-6544-B45F-8510F952AAF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7629A71C-C9E5-4E4F-BF55-2EA283741EDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="16940" xr2:uid="{BD53F7A6-3B44-6D46-90D6-01272792EFD4}"/>
   </bookViews>
@@ -129,45 +129,12 @@
     <t>Data/Images/brain.png</t>
   </si>
   <si>
-    <t>Data/Images/1_tail_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_tail_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_tail_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_tail_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_tail_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_gloves_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_gloves_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_gloves_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_gloves_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_gloves_5.png</t>
-  </si>
-  <si>
     <t>1_body</t>
   </si>
   <si>
     <t>2_body</t>
   </si>
   <si>
-    <t>Data/Images/2_body.png</t>
-  </si>
-  <si>
     <t>2_tail_1</t>
   </si>
   <si>
@@ -258,45 +225,6 @@
     <t>1_mou_5</t>
   </si>
   <si>
-    <t>Data/Images/1_eye_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_eye_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_eye_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_mou_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_mou_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_mou_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_mou_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_mou_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_ant_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_ant_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_ant_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_ant_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/1_ant_5.png</t>
-  </si>
-  <si>
     <t>2_arm_1</t>
   </si>
   <si>
@@ -372,99 +300,9 @@
     <t>2_ant_5</t>
   </si>
   <si>
-    <t>Data/Images/2_arm_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_arm_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_arm_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_arm_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_leg_1.png</t>
-  </si>
-  <si>
     <t>2_tail</t>
   </si>
   <si>
-    <t>Data/Images/2_tail.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_leg_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_leg_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_leg_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_leg_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_eye_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_eye_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_eye_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_eye_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_eye_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_mou_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_mou_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_mou_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_mou_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_mou_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_ant_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_ant_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_ant_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_ant_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_ant_5.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_tail_1.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_tail_2.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_tail_3.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_tail_4.png</t>
-  </si>
-  <si>
-    <t>Data/Images/2_tail_5.png</t>
-  </si>
-  <si>
     <t>Data/Images/Features_Placed/1_body.png</t>
   </si>
   <si>
@@ -502,6 +340,168 @@
   </si>
   <si>
     <t>Data/Images/Features_Placed/1_eye_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_eye_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_eye_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_eye_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_mou_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_mou_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_mou_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_mou_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_mou_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_ant_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_ant_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_ant_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_ant_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_ant_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_tail_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_tail_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_tail_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_tail_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_tail_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_gloves_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_gloves_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_gloves_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_gloves_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_gloves_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_body.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_arm_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_arm_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_arm_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_arm_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_leg_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_leg_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_leg_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_leg_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_leg_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_eye_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_eye_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_eye_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_eye_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_eye_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_mou_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_mou_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_mou_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_mou_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_mou_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_ant_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_ant_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_ant_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_ant_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_ant_5.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail_1.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail_2.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail_3.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail_4.png</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_tail_5.png</t>
   </si>
 </sst>
 </file>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D65F7A-FAAB-B447-AB7C-735700654342}">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,210 +924,210 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1143,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1151,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1159,7 +1159,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1167,7 +1167,7 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1175,7 +1175,7 @@
         <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1183,7 +1183,7 @@
         <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1191,7 +1191,7 @@
         <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1207,263 +1207,263 @@
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated assembly to assemble all aliens in procedure file
</commit_message>
<xml_diff>
--- a/Data/imagemap.xlsx
+++ b/Data/imagemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guest1\Documents\GitHub\Learning_Behavior_Aliens\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andywang/Desktop/Learning Behavior/Aliens/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E367A8-06FA-4532-9847-6979C4299422}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14BC9D3-BC55-9C4B-A193-61B09B71450F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD53F7A6-3B44-6D46-90D6-01272792EFD4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{BD53F7A6-3B44-6D46-90D6-01272792EFD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>Data/Images/Features_Placed/2_tail_5.png</t>
+  </si>
+  <si>
+    <t>2_skin</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/2_skin.png</t>
+  </si>
+  <si>
+    <t>1_skin</t>
+  </si>
+  <si>
+    <t>Data/Images/Features_Placed/1_skin.png</t>
   </si>
 </sst>
 </file>
@@ -859,20 +871,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D65F7A-FAAB-B447-AB7C-735700654342}">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="4" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -930,579 +942,595 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>64</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>65</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>66</v>
-      </c>
-      <c r="B41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>68</v>
       </c>
       <c r="B43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>69</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>70</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>71</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>72</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>73</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>74</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>75</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>76</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>77</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>78</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>79</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>80</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>81</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>82</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>83</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>84</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>85</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>86</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>87</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>88</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>89</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>34</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>35</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>36</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>37</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>38</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>2</v>
-      </c>
-      <c r="B70" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>4</v>
       </c>
       <c r="B72" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B73" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>6</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>